<commit_message>
adding and updating local explanation
</commit_message>
<xml_diff>
--- a/review/case_studyxlsx.xlsx
+++ b/review/case_studyxlsx.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22368" windowHeight="11928"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18468" windowHeight="9048"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,38 +494,93 @@
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="7"/>
+      <c r="B3" s="1">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="7"/>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="7"/>
+      <c r="B5">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="7"/>
+      <c r="B6">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="7">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>